<commit_message>
December 21, Today Latest Update
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/ProdCredentials.xlsx
+++ b/src/test/resources/Excel/ProdCredentials.xlsx
@@ -60,10 +60,10 @@
     <t>ExamDec12</t>
   </si>
   <si>
-    <t>jersey026.tt21.5</t>
-  </si>
-  <si>
     <t>F247A0</t>
+  </si>
+  <si>
+    <t>dec9.examtaker.5</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +461,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -476,7 +476,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>